<commit_message>
committing all work from Makuo
</commit_message>
<xml_diff>
--- a/GDP_data.xlsx
+++ b/GDP_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\makuo\NISR_Datathon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E26BF6A-52C2-4F6A-8F2D-409972A85C4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77923280-63BE-454C-B916-7298AC7D779B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D3CA5234-8822-4942-B4C0-1D6435CBB7DF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{D3CA5234-8822-4942-B4C0-1D6435CBB7DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Table A" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="76">
   <si>
     <t>GROSS DOMESTIC PRODUCT (GDP)</t>
   </si>
@@ -389,7 +389,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -452,6 +452,9 @@
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="171" fontId="4" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="170" fontId="4" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Comma 2 2" xfId="4" xr:uid="{AE40E49A-B263-4CCF-AF25-B2A468DCD73A}"/>
@@ -462,27 +465,7 @@
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
     <cellStyle name="Percent 2" xfId="6" xr:uid="{5B87446C-3AA3-4972-B1A7-BD90D707F11C}"/>
   </cellStyles>
-  <dxfs count="9">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
+  <dxfs count="5">
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
@@ -820,7 +803,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06C191C9-BC51-4137-B52E-ED0E5DD9ED44}">
   <dimension ref="A1:AE26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -3146,27 +3129,7 @@
     <row r="26" spans="1:31" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <conditionalFormatting sqref="R2:AE25">
-    <cfRule type="cellIs" dxfId="8" priority="3" stopIfTrue="1" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="V2 R2:U25">
-    <cfRule type="cellIs" dxfId="7" priority="7" stopIfTrue="1" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="V2 R2:U25">
-    <cfRule type="cellIs" dxfId="6" priority="6" stopIfTrue="1" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="V3:V25">
-    <cfRule type="cellIs" dxfId="5" priority="5" stopIfTrue="1" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="V3:V25">
-    <cfRule type="cellIs" dxfId="4" priority="4" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="3" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3178,7 +3141,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{428E41AE-16F0-437E-A60D-32A207833C8D}">
   <dimension ref="A1:AN26"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
@@ -6215,7 +6178,7 @@
   <dimension ref="A1:T27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7684,1074 +7647,1143 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FF152E4-7C0D-445C-B2A4-BF9AE83F2CEB}">
-  <dimension ref="A1:N25"/>
+  <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="14" max="14" width="13.88671875" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="46" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="C1" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="D1" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="E1" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="F1" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="G1" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="G1" s="23" t="s">
+      <c r="H1" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="I1" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="I1" s="24" t="s">
+      <c r="J1" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="J1" s="23" t="s">
+      <c r="K1" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="K1" s="23" t="s">
+      <c r="L1" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="L1" s="24" t="s">
+      <c r="M1" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="M1" s="23" t="s">
+      <c r="N1" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="N1" s="25" t="s">
+      <c r="O1" s="25" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="26">
+    <row r="2" spans="1:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="6">
+        <v>2000</v>
+      </c>
+      <c r="B2" s="26">
         <v>8.4000000000000005E-2</v>
       </c>
-      <c r="B2" s="27">
+      <c r="C2" s="27">
         <v>0.109</v>
       </c>
-      <c r="C2" s="28">
+      <c r="D2" s="28">
         <v>4.3999999999999997E-2</v>
       </c>
-      <c r="D2" s="28">
+      <c r="E2" s="28">
         <v>0.11799999999999999</v>
       </c>
-      <c r="E2" s="27">
+      <c r="F2" s="27">
         <v>0.16700000000000001</v>
       </c>
-      <c r="F2" s="29">
+      <c r="G2" s="29">
         <v>0.16700000000000001</v>
       </c>
-      <c r="G2" s="28">
+      <c r="H2" s="28">
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="H2" s="28">
+      <c r="I2" s="28">
         <v>0.42799999999999999</v>
       </c>
-      <c r="I2" s="29">
+      <c r="J2" s="29">
         <v>2E-3</v>
       </c>
-      <c r="J2" s="28">
+      <c r="K2" s="28">
         <v>6.2E-2</v>
       </c>
-      <c r="K2" s="28">
+      <c r="L2" s="28">
         <v>-9.1999999999999998E-2</v>
       </c>
-      <c r="L2" s="29">
+      <c r="M2" s="29">
         <v>0.245</v>
       </c>
-      <c r="M2" s="28">
+      <c r="N2" s="28">
         <v>0.16400000000000001</v>
       </c>
-      <c r="N2" s="30">
+      <c r="O2" s="30">
         <v>0.314</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="26">
+    <row r="3" spans="1:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="6">
+        <v>2001</v>
+      </c>
+      <c r="B3" s="26">
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="B3" s="27">
+      <c r="C3" s="27">
         <v>0.05</v>
       </c>
-      <c r="C3" s="28">
+      <c r="D3" s="28">
         <v>9.2999999999999999E-2</v>
       </c>
-      <c r="D3" s="28">
+      <c r="E3" s="28">
         <v>4.3999999999999997E-2</v>
       </c>
-      <c r="E3" s="27">
+      <c r="F3" s="27">
         <v>1E-3</v>
       </c>
-      <c r="F3" s="29">
+      <c r="G3" s="29">
         <v>1E-3</v>
       </c>
-      <c r="G3" s="28">
+      <c r="H3" s="28">
         <v>0.111</v>
       </c>
-      <c r="H3" s="28">
+      <c r="I3" s="28">
         <v>-0.161</v>
       </c>
-      <c r="I3" s="29">
+      <c r="J3" s="29">
         <v>0.39900000000000002</v>
       </c>
-      <c r="J3" s="28">
+      <c r="K3" s="28">
         <v>0.434</v>
       </c>
-      <c r="K3" s="28">
+      <c r="L3" s="28">
         <v>0.33500000000000002</v>
       </c>
-      <c r="L3" s="29">
+      <c r="M3" s="29">
         <v>-5.1999999999999998E-2</v>
       </c>
-      <c r="M3" s="28">
+      <c r="N3" s="28">
         <v>1.4E-2</v>
       </c>
-      <c r="N3" s="30">
+      <c r="O3" s="30">
         <v>-0.10199999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="26">
+    <row r="4" spans="1:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="6">
+        <v>2002</v>
+      </c>
+      <c r="B4" s="26">
         <v>0.13200000000000001</v>
       </c>
-      <c r="B4" s="27">
+      <c r="C4" s="27">
         <v>0.13700000000000001</v>
       </c>
-      <c r="C4" s="28">
+      <c r="D4" s="28">
         <v>0.14000000000000001</v>
       </c>
-      <c r="D4" s="28">
+      <c r="E4" s="28">
         <v>0.13600000000000001</v>
       </c>
-      <c r="E4" s="27">
+      <c r="F4" s="27">
         <v>7.6999999999999999E-2</v>
       </c>
-      <c r="F4" s="29">
+      <c r="G4" s="29">
         <v>7.6999999999999999E-2</v>
       </c>
-      <c r="G4" s="28">
+      <c r="H4" s="28">
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="H4" s="28">
+      <c r="I4" s="28">
         <v>0.121</v>
       </c>
-      <c r="I4" s="29">
+      <c r="J4" s="29">
         <v>5.0999999999999997E-2</v>
       </c>
-      <c r="J4" s="28">
+      <c r="K4" s="28">
         <v>-3.0000000000000001E-3</v>
       </c>
-      <c r="K4" s="28">
+      <c r="L4" s="28">
         <v>0.157</v>
       </c>
-      <c r="L4" s="29">
+      <c r="M4" s="29">
         <v>9.4E-2</v>
       </c>
-      <c r="M4" s="28">
+      <c r="N4" s="28">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="N4" s="30">
+      <c r="O4" s="30">
         <v>0.16400000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="26">
+    <row r="5" spans="1:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="6">
+        <v>2003</v>
+      </c>
+      <c r="B5" s="26">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="B5" s="27">
+      <c r="C5" s="27">
         <v>-2.4E-2</v>
       </c>
-      <c r="C5" s="28">
+      <c r="D5" s="28">
         <v>0.11799999999999999</v>
       </c>
-      <c r="D5" s="28">
+      <c r="E5" s="28">
         <v>-4.4999999999999998E-2</v>
       </c>
-      <c r="E5" s="27">
+      <c r="F5" s="27">
         <v>9.9000000000000005E-2</v>
       </c>
-      <c r="F5" s="29">
+      <c r="G5" s="29">
         <v>9.9000000000000005E-2</v>
       </c>
-      <c r="G5" s="28">
+      <c r="H5" s="28">
         <v>0.11899999999999999</v>
       </c>
-      <c r="H5" s="28">
+      <c r="I5" s="28">
         <v>6.3E-2</v>
       </c>
-      <c r="I5" s="29">
+      <c r="J5" s="29">
         <v>0.20399999999999999</v>
       </c>
-      <c r="J5" s="28">
+      <c r="K5" s="28">
         <v>-0.184</v>
       </c>
-      <c r="K5" s="28">
+      <c r="L5" s="28">
         <v>0.85499999999999998</v>
       </c>
-      <c r="L5" s="29">
+      <c r="M5" s="29">
         <v>-0.126</v>
       </c>
-      <c r="M5" s="28">
+      <c r="N5" s="28">
         <v>-0.123</v>
       </c>
-      <c r="N5" s="30">
+      <c r="O5" s="30">
         <v>-0.128</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="26">
+    <row r="6" spans="1:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="6">
+        <v>2004</v>
+      </c>
+      <c r="B6" s="26">
         <v>7.3999999999999996E-2</v>
       </c>
-      <c r="B6" s="27">
+      <c r="C6" s="27">
         <v>7.0999999999999994E-2</v>
       </c>
-      <c r="C6" s="28">
+      <c r="D6" s="28">
         <v>9.6000000000000002E-2</v>
       </c>
-      <c r="D6" s="28">
+      <c r="E6" s="28">
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="E6" s="27">
+      <c r="F6" s="27">
         <v>0.11899999999999999</v>
       </c>
-      <c r="F6" s="29">
+      <c r="G6" s="29">
         <v>0.11899999999999999</v>
       </c>
-      <c r="G6" s="28">
+      <c r="H6" s="28">
         <v>0.253</v>
       </c>
-      <c r="H6" s="28">
+      <c r="I6" s="28">
         <v>-0.13900000000000001</v>
       </c>
-      <c r="I6" s="29">
+      <c r="J6" s="29">
         <v>0.317</v>
       </c>
-      <c r="J6" s="28">
+      <c r="K6" s="28">
         <v>0.20399999999999999</v>
       </c>
-      <c r="K6" s="28">
+      <c r="L6" s="28">
         <v>0.40100000000000002</v>
       </c>
-      <c r="L6" s="29">
+      <c r="M6" s="29">
         <v>0.21</v>
       </c>
-      <c r="M6" s="28">
+      <c r="N6" s="28">
         <v>0.23400000000000001</v>
       </c>
-      <c r="N6" s="30">
+      <c r="O6" s="30">
         <v>0.192</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="26">
+    <row r="7" spans="1:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="6">
+        <v>2005</v>
+      </c>
+      <c r="B7" s="26">
         <v>9.4E-2</v>
       </c>
-      <c r="B7" s="27">
+      <c r="C7" s="27">
         <v>8.7999999999999995E-2</v>
       </c>
-      <c r="C7" s="28">
+      <c r="D7" s="28">
         <v>9.5000000000000001E-2</v>
       </c>
-      <c r="D7" s="28">
+      <c r="E7" s="28">
         <v>8.6999999999999994E-2</v>
       </c>
-      <c r="E7" s="27">
+      <c r="F7" s="27">
         <v>0.161</v>
       </c>
-      <c r="F7" s="29">
+      <c r="G7" s="29">
         <v>0.161</v>
       </c>
-      <c r="G7" s="28">
+      <c r="H7" s="28">
         <v>0.125</v>
       </c>
-      <c r="H7" s="28">
+      <c r="I7" s="28">
         <v>0.25900000000000001</v>
       </c>
-      <c r="I7" s="29">
+      <c r="J7" s="29">
         <v>0.112</v>
       </c>
-      <c r="J7" s="28">
+      <c r="K7" s="28">
         <v>9.0999999999999998E-2</v>
       </c>
-      <c r="K7" s="28">
+      <c r="L7" s="28">
         <v>0.125</v>
       </c>
-      <c r="L7" s="29">
+      <c r="M7" s="29">
         <v>0.11799999999999999</v>
       </c>
-      <c r="M7" s="28">
+      <c r="N7" s="28">
         <v>0.17699999999999999</v>
       </c>
-      <c r="N7" s="30">
+      <c r="O7" s="30">
         <v>7.2999999999999995E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="26">
+    <row r="8" spans="1:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="6">
+        <v>2006</v>
+      </c>
+      <c r="B8" s="26">
         <v>9.1999999999999998E-2</v>
       </c>
-      <c r="B8" s="27">
+      <c r="C8" s="27">
         <v>0.10100000000000001</v>
       </c>
-      <c r="C8" s="28">
+      <c r="D8" s="28">
         <v>9.4E-2</v>
       </c>
-      <c r="D8" s="28">
+      <c r="E8" s="28">
         <v>0.10199999999999999</v>
       </c>
-      <c r="E8" s="27">
+      <c r="F8" s="27">
         <v>0.28599999999999998</v>
       </c>
-      <c r="F8" s="29">
+      <c r="G8" s="29">
         <v>0.24399999999999999</v>
       </c>
-      <c r="G8" s="28">
+      <c r="H8" s="28">
         <v>0.221</v>
       </c>
-      <c r="H8" s="28">
+      <c r="I8" s="28">
         <v>0.29299999999999998</v>
       </c>
-      <c r="I8" s="29">
+      <c r="J8" s="29">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="J8" s="28">
+      <c r="K8" s="28">
         <v>-1E-3</v>
       </c>
-      <c r="K8" s="28">
+      <c r="L8" s="28">
         <v>4.9000000000000002E-2</v>
       </c>
-      <c r="L8" s="29">
+      <c r="M8" s="29">
         <v>0.23400000000000001</v>
       </c>
-      <c r="M8" s="28">
+      <c r="N8" s="28">
         <v>0.32300000000000001</v>
       </c>
-      <c r="N8" s="30">
+      <c r="O8" s="30">
         <v>0.26500000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="26">
+    <row r="9" spans="1:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="6">
+        <v>2007</v>
+      </c>
+      <c r="B9" s="26">
         <v>7.5999999999999998E-2</v>
       </c>
-      <c r="B9" s="27">
+      <c r="C9" s="27">
         <v>2.3E-2</v>
       </c>
-      <c r="C9" s="28">
+      <c r="D9" s="28">
         <v>1.2E-2</v>
       </c>
-      <c r="D9" s="28">
+      <c r="E9" s="28">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="E9" s="27">
+      <c r="F9" s="27">
         <v>0.26900000000000002</v>
       </c>
-      <c r="F9" s="29">
+      <c r="G9" s="29">
         <v>0.27700000000000002</v>
       </c>
-      <c r="G9" s="28">
+      <c r="H9" s="28">
         <v>0.156</v>
       </c>
-      <c r="H9" s="28">
+      <c r="I9" s="28">
         <v>0.53400000000000003</v>
       </c>
-      <c r="I9" s="29">
+      <c r="J9" s="29">
         <v>0.44</v>
       </c>
-      <c r="J9" s="28">
+      <c r="K9" s="28">
         <v>0.156</v>
       </c>
-      <c r="K9" s="28">
+      <c r="L9" s="28">
         <v>0.61599999999999999</v>
       </c>
-      <c r="L9" s="29">
+      <c r="M9" s="29">
         <v>0.124</v>
       </c>
-      <c r="M9" s="28">
+      <c r="N9" s="28">
         <v>0.255</v>
       </c>
-      <c r="N9" s="30">
+      <c r="O9" s="30">
         <v>-1.4E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="26">
+    <row r="10" spans="1:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="6">
+        <v>2008</v>
+      </c>
+      <c r="B10" s="26">
         <v>0.112</v>
       </c>
-      <c r="B10" s="27">
+      <c r="C10" s="27">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="C10" s="28">
+      <c r="D10" s="28">
         <v>2.3E-2</v>
       </c>
-      <c r="D10" s="28">
+      <c r="E10" s="28">
         <v>7.8E-2</v>
       </c>
-      <c r="E10" s="27">
+      <c r="F10" s="27">
         <v>0.32</v>
       </c>
-      <c r="F10" s="29">
+      <c r="G10" s="29">
         <v>0.32700000000000001</v>
       </c>
-      <c r="G10" s="28">
+      <c r="H10" s="28">
         <v>0.29499999999999998</v>
       </c>
-      <c r="H10" s="28">
+      <c r="I10" s="28">
         <v>0.379</v>
       </c>
-      <c r="I10" s="29">
+      <c r="J10" s="29">
         <v>-0.114</v>
       </c>
-      <c r="J10" s="28">
+      <c r="K10" s="28">
         <v>0.25900000000000001</v>
       </c>
-      <c r="K10" s="28">
+      <c r="L10" s="28">
         <v>-0.28000000000000003</v>
       </c>
-      <c r="L10" s="29">
+      <c r="M10" s="29">
         <v>-2.7E-2</v>
       </c>
-      <c r="M10" s="28">
+      <c r="N10" s="28">
         <v>0.18</v>
       </c>
-      <c r="N10" s="30">
+      <c r="O10" s="30">
         <v>-0.30599999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="26">
+    <row r="11" spans="1:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="6">
+        <v>2009</v>
+      </c>
+      <c r="B11" s="26">
         <v>6.2E-2</v>
       </c>
-      <c r="B11" s="27">
+      <c r="C11" s="27">
         <v>0.10100000000000001</v>
       </c>
-      <c r="C11" s="28">
+      <c r="D11" s="28">
         <v>0.11600000000000001</v>
       </c>
-      <c r="D11" s="28">
+      <c r="E11" s="28">
         <v>9.9000000000000005E-2</v>
       </c>
-      <c r="E11" s="27">
+      <c r="F11" s="27">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="F11" s="29">
+      <c r="G11" s="29">
         <v>2.7E-2</v>
       </c>
-      <c r="G11" s="28">
+      <c r="H11" s="28">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="H11" s="28">
+      <c r="I11" s="28">
         <v>4.2999999999999997E-2</v>
       </c>
-      <c r="I11" s="29">
+      <c r="J11" s="29">
         <v>-3.1E-2</v>
       </c>
-      <c r="J11" s="28">
+      <c r="K11" s="28">
         <v>-0.27300000000000002</v>
       </c>
-      <c r="K11" s="28">
+      <c r="L11" s="28">
         <v>0.156</v>
       </c>
-      <c r="L11" s="29">
+      <c r="M11" s="29">
         <v>0.17199999999999999</v>
       </c>
-      <c r="M11" s="28">
+      <c r="N11" s="28">
         <v>0.151</v>
       </c>
-      <c r="N11" s="30">
+      <c r="O11" s="30">
         <v>0.218</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="26">
+    <row r="12" spans="1:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="6">
+        <v>2010</v>
+      </c>
+      <c r="B12" s="26">
         <v>7.2999999999999995E-2</v>
       </c>
-      <c r="B12" s="27">
+      <c r="C12" s="27">
         <v>6.2E-2</v>
       </c>
-      <c r="C12" s="28">
+      <c r="D12" s="28">
         <v>0.104</v>
       </c>
-      <c r="D12" s="28">
+      <c r="E12" s="28">
         <v>5.6000000000000001E-2</v>
       </c>
-      <c r="E12" s="27">
+      <c r="F12" s="27">
         <v>7.0999999999999994E-2</v>
       </c>
-      <c r="F12" s="29">
+      <c r="G12" s="29">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="G12" s="28">
+      <c r="H12" s="28">
         <v>9.0999999999999998E-2</v>
       </c>
-      <c r="H12" s="28">
+      <c r="I12" s="28">
         <v>0.04</v>
       </c>
-      <c r="I12" s="29">
+      <c r="J12" s="29">
         <v>8.2000000000000003E-2</v>
       </c>
-      <c r="J12" s="28">
+      <c r="K12" s="28">
         <v>0.28799999999999998</v>
       </c>
-      <c r="K12" s="28">
+      <c r="L12" s="28">
         <v>-1.7999999999999999E-2</v>
       </c>
-      <c r="L12" s="29">
+      <c r="M12" s="29">
         <v>2.3E-2</v>
       </c>
-      <c r="M12" s="28">
+      <c r="N12" s="28">
         <v>9.2999999999999999E-2</v>
       </c>
-      <c r="N12" s="30">
+      <c r="O12" s="30">
         <v>-0.129</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="26">
+    <row r="13" spans="1:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="6">
+        <v>2011</v>
+      </c>
+      <c r="B13" s="26">
         <v>0.08</v>
       </c>
-      <c r="B13" s="27">
+      <c r="C13" s="27">
         <v>8.2000000000000003E-2</v>
       </c>
-      <c r="C13" s="28">
+      <c r="D13" s="28">
         <v>3.9E-2</v>
       </c>
-      <c r="D13" s="28">
+      <c r="E13" s="28">
         <v>0.09</v>
       </c>
-      <c r="E13" s="27">
+      <c r="F13" s="27">
         <v>9.2999999999999999E-2</v>
       </c>
-      <c r="F13" s="29">
+      <c r="G13" s="29">
         <v>9.2999999999999999E-2</v>
       </c>
-      <c r="G13" s="28">
+      <c r="H13" s="28">
         <v>0.245</v>
       </c>
-      <c r="H13" s="28">
+      <c r="I13" s="28">
         <v>-0.14099999999999999</v>
       </c>
-      <c r="I13" s="29">
+      <c r="J13" s="29">
         <v>0.23699999999999999</v>
       </c>
-      <c r="J13" s="28">
+      <c r="K13" s="28">
         <v>0.621</v>
       </c>
-      <c r="K13" s="28">
+      <c r="L13" s="28">
         <v>-1.0999999999999999E-2</v>
       </c>
-      <c r="L13" s="29">
+      <c r="M13" s="29">
         <v>0.17699999999999999</v>
       </c>
-      <c r="M13" s="28">
+      <c r="N13" s="28">
         <v>0.20300000000000001</v>
       </c>
-      <c r="N13" s="30">
+      <c r="O13" s="30">
         <v>0.109</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="26">
+    <row r="14" spans="1:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="6">
+        <v>2012</v>
+      </c>
+      <c r="B14" s="26">
         <v>8.5999999999999993E-2</v>
       </c>
-      <c r="B14" s="27">
+      <c r="C14" s="27">
         <v>7.9000000000000001E-2</v>
       </c>
-      <c r="C14" s="28">
+      <c r="D14" s="28">
         <v>0.158</v>
       </c>
-      <c r="D14" s="28">
+      <c r="E14" s="28">
         <v>6.6000000000000003E-2</v>
       </c>
-      <c r="E14" s="27">
+      <c r="F14" s="27">
         <v>0.223</v>
       </c>
-      <c r="F14" s="29">
+      <c r="G14" s="29">
         <v>0.219</v>
       </c>
-      <c r="G14" s="28">
+      <c r="H14" s="28">
         <v>0.154</v>
       </c>
-      <c r="H14" s="28">
+      <c r="I14" s="28">
         <v>0.36</v>
       </c>
-      <c r="I14" s="29">
+      <c r="J14" s="29">
         <v>0.09</v>
       </c>
-      <c r="J14" s="28">
+      <c r="K14" s="28">
         <v>0.22900000000000001</v>
       </c>
-      <c r="K14" s="28">
+      <c r="L14" s="28">
         <v>-5.0999999999999997E-2</v>
       </c>
-      <c r="L14" s="29">
+      <c r="M14" s="29">
         <v>0.188</v>
       </c>
-      <c r="M14" s="28">
+      <c r="N14" s="28">
         <v>0.22700000000000001</v>
       </c>
-      <c r="N14" s="30">
+      <c r="O14" s="30">
         <v>6.8000000000000005E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="26">
+    <row r="15" spans="1:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="6">
+        <v>2013</v>
+      </c>
+      <c r="B15" s="26">
         <v>4.7E-2</v>
       </c>
-      <c r="B15" s="27">
+      <c r="C15" s="27">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="C15" s="28">
+      <c r="D15" s="28">
         <v>-2E-3</v>
       </c>
-      <c r="D15" s="28">
+      <c r="E15" s="28">
         <v>4.2000000000000003E-2</v>
       </c>
-      <c r="E15" s="27">
+      <c r="F15" s="27">
         <v>7.6999999999999999E-2</v>
       </c>
-      <c r="F15" s="29">
+      <c r="G15" s="29">
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="G15" s="28">
+      <c r="H15" s="28">
         <v>0.113</v>
       </c>
-      <c r="H15" s="28">
+      <c r="I15" s="28">
         <v>0</v>
       </c>
-      <c r="I15" s="29">
+      <c r="J15" s="29">
         <v>0.189</v>
       </c>
-      <c r="J15" s="28">
+      <c r="K15" s="28">
         <v>0.24399999999999999</v>
       </c>
-      <c r="K15" s="28">
+      <c r="L15" s="28">
         <v>0.112</v>
       </c>
-      <c r="L15" s="29">
+      <c r="M15" s="29">
         <v>9.0999999999999998E-2</v>
       </c>
-      <c r="M15" s="28">
+      <c r="N15" s="28">
         <v>5.8000000000000003E-2</v>
       </c>
-      <c r="N15" s="30">
+      <c r="O15" s="30">
         <v>0.20599999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="26">
+    <row r="16" spans="1:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="6">
+        <v>2014</v>
+      </c>
+      <c r="B16" s="26">
         <v>6.2E-2</v>
       </c>
-      <c r="B16" s="27">
+      <c r="C16" s="27">
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="C16" s="28">
+      <c r="D16" s="28">
         <v>0.20699999999999999</v>
       </c>
-      <c r="D16" s="28">
+      <c r="E16" s="28">
         <v>6.4000000000000001E-2</v>
       </c>
-      <c r="E16" s="27">
+      <c r="F16" s="27">
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="F16" s="29">
+      <c r="G16" s="29">
         <v>4.9000000000000002E-2</v>
       </c>
-      <c r="G16" s="28">
+      <c r="H16" s="28">
         <v>5.1999999999999998E-2</v>
       </c>
-      <c r="H16" s="28">
+      <c r="I16" s="28">
         <v>4.1000000000000002E-2</v>
       </c>
-      <c r="I16" s="29">
+      <c r="J16" s="29">
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="J16" s="28">
+      <c r="K16" s="28">
         <v>-9.4E-2</v>
       </c>
-      <c r="K16" s="28">
+      <c r="L16" s="28">
         <v>0.311</v>
       </c>
-      <c r="L16" s="29">
+      <c r="M16" s="29">
         <v>0.14599999999999999</v>
       </c>
-      <c r="M16" s="28">
+      <c r="N16" s="28">
         <v>0.13100000000000001</v>
       </c>
-      <c r="N16" s="30">
+      <c r="O16" s="30">
         <v>0.182</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="26">
+    <row r="17" spans="1:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="6">
+        <v>2015</v>
+      </c>
+      <c r="B17" s="26">
         <v>8.8999999999999996E-2</v>
       </c>
-      <c r="B17" s="27">
+      <c r="C17" s="27">
         <v>0.109</v>
       </c>
-      <c r="C17" s="28">
+      <c r="D17" s="28">
         <v>5.0999999999999997E-2</v>
       </c>
-      <c r="D17" s="28">
+      <c r="E17" s="28">
         <v>0.12</v>
       </c>
-      <c r="E17" s="27">
+      <c r="F17" s="27">
         <v>0.17899999999999999</v>
       </c>
-      <c r="F17" s="29">
+      <c r="G17" s="29">
         <v>0.188</v>
       </c>
-      <c r="G17" s="28">
+      <c r="H17" s="28">
         <v>0.157</v>
       </c>
-      <c r="H17" s="28">
+      <c r="I17" s="28">
         <v>0.26600000000000001</v>
       </c>
-      <c r="I17" s="29">
+      <c r="J17" s="29">
         <v>6.3E-2</v>
       </c>
-      <c r="J17" s="28">
+      <c r="K17" s="28">
         <v>-1.9E-2</v>
       </c>
-      <c r="K17" s="28">
+      <c r="L17" s="28">
         <v>0.14399999999999999</v>
       </c>
-      <c r="L17" s="29">
+      <c r="M17" s="29">
         <v>0.23</v>
       </c>
-      <c r="M17" s="28">
+      <c r="N17" s="28">
         <v>0.114</v>
       </c>
-      <c r="N17" s="30">
+      <c r="O17" s="30">
         <v>0.505</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="26">
+    <row r="18" spans="1:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="6">
+        <v>2016</v>
+      </c>
+      <c r="B18" s="26">
         <v>0.06</v>
       </c>
-      <c r="B18" s="27">
+      <c r="C18" s="27">
         <v>0.05</v>
       </c>
-      <c r="C18" s="28">
+      <c r="D18" s="28">
         <v>9.1999999999999998E-2</v>
       </c>
-      <c r="D18" s="28">
+      <c r="E18" s="28">
         <v>4.2000000000000003E-2</v>
       </c>
-      <c r="E18" s="27">
+      <c r="F18" s="27">
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="F18" s="29">
+      <c r="G18" s="29">
         <v>0.09</v>
       </c>
-      <c r="G18" s="28">
+      <c r="H18" s="28">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="H18" s="28">
+      <c r="I18" s="28">
         <v>0.23799999999999999</v>
       </c>
-      <c r="I18" s="29">
+      <c r="J18" s="29">
         <v>0.129</v>
       </c>
-      <c r="J18" s="28">
+      <c r="K18" s="28">
         <v>0.104</v>
       </c>
-      <c r="K18" s="28">
+      <c r="L18" s="28">
         <v>0.151</v>
       </c>
-      <c r="L18" s="29">
+      <c r="M18" s="29">
         <v>7.5999999999999998E-2</v>
       </c>
-      <c r="M18" s="28">
+      <c r="N18" s="28">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="N18" s="30">
+      <c r="O18" s="30">
         <v>8.7999999999999995E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="26">
+    <row r="19" spans="1:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="6">
+        <v>2017</v>
+      </c>
+      <c r="B19" s="26">
         <v>3.9E-2</v>
       </c>
-      <c r="B19" s="27">
+      <c r="C19" s="27">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="C19" s="28">
+      <c r="D19" s="28">
         <v>7.2999999999999995E-2</v>
       </c>
-      <c r="D19" s="28">
+      <c r="E19" s="28">
         <v>-7.0000000000000001E-3</v>
       </c>
-      <c r="E19" s="27">
+      <c r="F19" s="27">
         <v>-4.4999999999999998E-2</v>
       </c>
-      <c r="F19" s="29">
+      <c r="G19" s="29">
         <v>-0.10199999999999999</v>
       </c>
-      <c r="G19" s="28">
+      <c r="H19" s="28">
         <v>-9.8000000000000004E-2</v>
       </c>
-      <c r="H19" s="28">
+      <c r="I19" s="28">
         <v>-0.11</v>
       </c>
-      <c r="I19" s="29">
+      <c r="J19" s="29">
         <v>0.433</v>
       </c>
-      <c r="J19" s="28">
+      <c r="K19" s="28">
         <v>1.1020000000000001</v>
       </c>
-      <c r="K19" s="28">
+      <c r="L19" s="28">
         <v>4.2999999999999997E-2</v>
       </c>
-      <c r="L19" s="29">
+      <c r="M19" s="29">
         <v>5.8000000000000003E-2</v>
       </c>
-      <c r="M19" s="28">
+      <c r="N19" s="28">
         <v>9.7000000000000003E-2</v>
       </c>
-      <c r="N19" s="30">
+      <c r="O19" s="30">
         <v>-8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="26">
+    <row r="20" spans="1:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="6">
+        <v>2018</v>
+      </c>
+      <c r="B20" s="26">
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="B20" s="27">
+      <c r="C20" s="27">
         <v>0.10199999999999999</v>
       </c>
-      <c r="C20" s="28">
+      <c r="D20" s="28">
         <v>0.05</v>
       </c>
-      <c r="D20" s="28">
+      <c r="E20" s="28">
         <v>0.112</v>
       </c>
-      <c r="E20" s="27">
+      <c r="F20" s="27">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="F20" s="29">
+      <c r="G20" s="29">
         <v>0.06</v>
       </c>
-      <c r="G20" s="28">
+      <c r="H20" s="28">
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="H20" s="28">
+      <c r="I20" s="28">
         <v>8.4000000000000005E-2</v>
       </c>
-      <c r="I20" s="29">
+      <c r="J20" s="29">
         <v>0.10199999999999999</v>
       </c>
-      <c r="J20" s="28">
+      <c r="K20" s="28">
         <v>0.12</v>
       </c>
-      <c r="K20" s="28">
+      <c r="L20" s="28">
         <v>8.1000000000000003E-2</v>
       </c>
-      <c r="L20" s="29">
+      <c r="M20" s="29">
         <v>8.1000000000000003E-2</v>
       </c>
-      <c r="M20" s="28">
+      <c r="N20" s="28">
         <v>0.128</v>
       </c>
-      <c r="N20" s="30">
+      <c r="O20" s="30">
         <v>-8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="26">
+    <row r="21" spans="1:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="6">
+        <v>2019</v>
+      </c>
+      <c r="B21" s="26">
         <v>9.5000000000000001E-2</v>
       </c>
-      <c r="B21" s="27">
+      <c r="C21" s="27">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="C21" s="28">
+      <c r="D21" s="28">
         <v>0.17599999999999999</v>
       </c>
-      <c r="D21" s="28">
+      <c r="E21" s="28">
         <v>5.5E-2</v>
       </c>
-      <c r="E21" s="27">
+      <c r="F21" s="27">
         <v>0.20699999999999999</v>
       </c>
-      <c r="F21" s="29">
+      <c r="G21" s="29">
         <v>0.32100000000000001</v>
       </c>
-      <c r="G21" s="28">
+      <c r="H21" s="28">
         <v>0.32800000000000001</v>
       </c>
-      <c r="H21" s="28">
+      <c r="I21" s="28">
         <v>0.30599999999999999</v>
       </c>
-      <c r="I21" s="29">
+      <c r="J21" s="29">
         <v>0.19900000000000001</v>
       </c>
-      <c r="J21" s="28">
+      <c r="K21" s="28">
         <v>0.255</v>
       </c>
-      <c r="K21" s="28">
+      <c r="L21" s="28">
         <v>0.13</v>
       </c>
-      <c r="L21" s="29">
+      <c r="M21" s="29">
         <v>0.18099999999999999</v>
       </c>
-      <c r="M21" s="28">
+      <c r="N21" s="28">
         <v>0.25</v>
       </c>
-      <c r="N21" s="30">
+      <c r="O21" s="30">
         <v>3.2000000000000001E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="26">
+    <row r="22" spans="1:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="6">
+        <v>2020</v>
+      </c>
+      <c r="B22" s="26">
         <v>-3.4000000000000002E-2</v>
       </c>
-      <c r="B22" s="27">
+      <c r="C22" s="27">
         <v>-3.7999999999999999E-2</v>
       </c>
-      <c r="C22" s="28">
+      <c r="D22" s="28">
         <v>1.9E-2</v>
       </c>
-      <c r="D22" s="28">
+      <c r="E22" s="28">
         <v>-0.05</v>
       </c>
-      <c r="E22" s="27">
+      <c r="F22" s="27">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="F22" s="29">
+      <c r="G22" s="29">
         <v>-4.4999999999999998E-2</v>
       </c>
-      <c r="G22" s="28">
+      <c r="H22" s="28">
         <v>-5.7000000000000002E-2</v>
       </c>
-      <c r="H22" s="28">
+      <c r="I22" s="28">
         <v>-2.3E-2</v>
       </c>
-      <c r="I22" s="29">
+      <c r="J22" s="29">
         <v>-9.1999999999999998E-2</v>
       </c>
-      <c r="J22" s="28">
+      <c r="K22" s="28">
         <v>0.21199999999999999</v>
       </c>
-      <c r="K22" s="28">
+      <c r="L22" s="28">
         <v>-0.502</v>
       </c>
-      <c r="L22" s="29">
+      <c r="M22" s="29">
         <v>-3.4000000000000002E-2</v>
       </c>
-      <c r="M22" s="28">
+      <c r="N22" s="28">
         <v>0.13300000000000001</v>
       </c>
-      <c r="N22" s="30">
+      <c r="O22" s="30">
         <v>-0.47399999999999998</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="26">
+    <row r="23" spans="1:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="6">
+        <v>2021</v>
+      </c>
+      <c r="B23" s="26">
         <v>0.109</v>
       </c>
-      <c r="B23" s="27">
+      <c r="C23" s="27">
         <v>9.7000000000000003E-2</v>
       </c>
-      <c r="C23" s="28">
+      <c r="D23" s="28">
         <v>0.13700000000000001</v>
       </c>
-      <c r="D23" s="28">
+      <c r="E23" s="28">
         <v>8.7999999999999995E-2</v>
       </c>
-      <c r="E23" s="27">
+      <c r="F23" s="27">
         <v>0.114</v>
       </c>
-      <c r="F23" s="29">
+      <c r="G23" s="29">
         <v>0.16500000000000001</v>
       </c>
-      <c r="G23" s="28">
+      <c r="H23" s="28">
         <v>0.152</v>
       </c>
-      <c r="H23" s="28">
+      <c r="I23" s="28">
         <v>0.19</v>
       </c>
-      <c r="I23" s="29">
+      <c r="J23" s="29">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="J23" s="28">
+      <c r="K23" s="28">
         <v>-4.7E-2</v>
       </c>
-      <c r="K23" s="28">
+      <c r="L23" s="28">
         <v>0.27600000000000002</v>
       </c>
-      <c r="L23" s="29">
+      <c r="M23" s="29">
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="M23" s="28">
+      <c r="N23" s="28">
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="N23" s="30">
+      <c r="O23" s="30">
         <v>0.06</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="26">
+    <row r="24" spans="1:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="6">
+        <v>2022</v>
+      </c>
+      <c r="B24" s="26">
         <v>8.2000000000000003E-2</v>
       </c>
-      <c r="B24" s="27">
+      <c r="C24" s="27">
         <v>0.11600000000000001</v>
       </c>
-      <c r="C24" s="28">
+      <c r="D24" s="28">
         <v>0.106</v>
       </c>
-      <c r="D24" s="28">
+      <c r="E24" s="28">
         <v>0.11899999999999999</v>
       </c>
-      <c r="E24" s="27">
+      <c r="F24" s="27">
         <v>-0.10100000000000001</v>
       </c>
-      <c r="F24" s="29">
+      <c r="G24" s="29">
         <v>-4.2000000000000003E-2</v>
       </c>
-      <c r="G24" s="28">
+      <c r="H24" s="28">
         <v>-5.7000000000000002E-2</v>
       </c>
-      <c r="H24" s="28">
+      <c r="I24" s="28">
         <v>-1.4999999999999999E-2</v>
       </c>
-      <c r="I24" s="29">
+      <c r="J24" s="29">
         <v>0.30099999999999999</v>
       </c>
-      <c r="J24" s="28">
+      <c r="K24" s="28">
         <v>0.32900000000000001</v>
       </c>
-      <c r="K24" s="28">
+      <c r="L24" s="28">
         <v>0.23400000000000001</v>
       </c>
-      <c r="L24" s="29">
+      <c r="M24" s="29">
         <v>0.161</v>
       </c>
-      <c r="M24" s="28">
+      <c r="N24" s="28">
         <v>0.12</v>
       </c>
-      <c r="N24" s="30">
+      <c r="O24" s="30">
         <v>0.38400000000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="1:15" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
updating GDP data sheet
</commit_message>
<xml_diff>
--- a/GDP_data.xlsx
+++ b/GDP_data.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\makuo\NISR_Datathon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77923280-63BE-454C-B916-7298AC7D779B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F40BE9CA-53EC-4BDE-8C03-485CB1F045EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{D3CA5234-8822-4942-B4C0-1D6435CBB7DF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{D3CA5234-8822-4942-B4C0-1D6435CBB7DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Table A" sheetId="1" r:id="rId1"/>
     <sheet name="CYGDP KP" sheetId="2" r:id="rId2"/>
     <sheet name="T3 GDP CY" sheetId="3" r:id="rId3"/>
     <sheet name="T3A GDP XCY" sheetId="4" r:id="rId4"/>
+    <sheet name="CYGDP Gr" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="76">
   <si>
     <t>GROSS DOMESTIC PRODUCT (GDP)</t>
   </si>
@@ -389,7 +390,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -455,6 +456,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="168" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Comma 2 2" xfId="4" xr:uid="{AE40E49A-B263-4CCF-AF25-B2A468DCD73A}"/>
@@ -7649,7 +7655,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FF152E4-7C0D-445C-B2A4-BF9AE83F2CEB}">
   <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
@@ -8788,4 +8794,2876 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1A59DDE-C4BF-4F33-89C1-56B65A84F3C1}">
+  <dimension ref="A1:AM25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:39" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="AG1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AH1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="AI1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="AJ1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="AK1" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="AL1" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="AM1" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:39" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="6">
+        <v>2000</v>
+      </c>
+      <c r="B2" s="47">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="C2" s="48">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="D2" s="49">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="E2" s="49">
+        <v>0.16200000000000001</v>
+      </c>
+      <c r="F2" s="49">
+        <v>0.05</v>
+      </c>
+      <c r="G2" s="49">
+        <v>0.05</v>
+      </c>
+      <c r="H2" s="49">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="I2" s="48">
+        <v>1.6E-2</v>
+      </c>
+      <c r="J2" s="49">
+        <v>0.40799999999999997</v>
+      </c>
+      <c r="K2" s="50">
+        <v>-2E-3</v>
+      </c>
+      <c r="L2" s="51">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="M2" s="51">
+        <v>-0.08</v>
+      </c>
+      <c r="N2" s="51">
+        <v>0.17</v>
+      </c>
+      <c r="O2" s="51">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="P2" s="51">
+        <v>-1E-3</v>
+      </c>
+      <c r="Q2" s="51">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="R2" s="51">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="S2" s="51">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="T2" s="49">
+        <v>-0.114</v>
+      </c>
+      <c r="U2" s="49">
+        <v>-0.114</v>
+      </c>
+      <c r="V2" s="49">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="W2" s="48">
+        <v>0.115</v>
+      </c>
+      <c r="X2" s="48">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="Y2" s="49">
+        <v>0.13</v>
+      </c>
+      <c r="Z2" s="49">
+        <v>0.13</v>
+      </c>
+      <c r="AA2" s="49">
+        <v>0.16</v>
+      </c>
+      <c r="AB2" s="48">
+        <v>0.125</v>
+      </c>
+      <c r="AC2" s="49">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="AD2" s="49">
+        <v>0.16</v>
+      </c>
+      <c r="AE2" s="49">
+        <v>0.223</v>
+      </c>
+      <c r="AF2" s="49">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="AG2" s="49">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="AH2" s="49">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="AI2" s="49">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="AJ2" s="49">
+        <v>0.182</v>
+      </c>
+      <c r="AK2" s="49">
+        <v>2.3E-2</v>
+      </c>
+      <c r="AL2" s="49">
+        <v>4.1749999999999998</v>
+      </c>
+      <c r="AM2" s="48">
+        <v>8.4000000000000005E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:39" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="6">
+        <v>2001</v>
+      </c>
+      <c r="B3" s="47">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="C3" s="48">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="D3" s="49">
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="E3" s="49">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="F3" s="49">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="G3" s="49">
+        <v>0.08</v>
+      </c>
+      <c r="H3" s="49">
+        <v>0.08</v>
+      </c>
+      <c r="I3" s="48">
+        <v>0.129</v>
+      </c>
+      <c r="J3" s="49">
+        <v>1.7230000000000001</v>
+      </c>
+      <c r="K3" s="50">
+        <v>0.1</v>
+      </c>
+      <c r="L3" s="51">
+        <v>0.247</v>
+      </c>
+      <c r="M3" s="51">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="N3" s="51">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="O3" s="51">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="P3" s="51">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="Q3" s="51">
+        <v>0.24399999999999999</v>
+      </c>
+      <c r="R3" s="51">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="S3" s="51">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="T3" s="49">
+        <v>-9.9000000000000005E-2</v>
+      </c>
+      <c r="U3" s="49">
+        <v>-9.9000000000000005E-2</v>
+      </c>
+      <c r="V3" s="49">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="W3" s="48">
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="X3" s="48">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="Y3" s="49">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="Z3" s="49">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="AA3" s="49">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="AB3" s="48">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="AC3" s="49">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="AD3" s="49">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="AE3" s="49">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="AF3" s="49">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="AG3" s="49">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="AH3" s="49">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="AI3" s="49">
+        <v>3.9E-2</v>
+      </c>
+      <c r="AJ3" s="49">
+        <v>0.122</v>
+      </c>
+      <c r="AK3" s="49">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="AL3" s="49">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="AM3" s="48">
+        <v>8.5000000000000006E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:39" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="6">
+        <v>2002</v>
+      </c>
+      <c r="B4" s="47">
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="C4" s="48">
+        <v>0.16900000000000001</v>
+      </c>
+      <c r="D4" s="49">
+        <v>0.187</v>
+      </c>
+      <c r="E4" s="49">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="F4" s="49">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="G4" s="49">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="H4" s="49">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="I4" s="48">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="J4" s="49">
+        <v>-0.24199999999999999</v>
+      </c>
+      <c r="K4" s="50">
+        <v>0.152</v>
+      </c>
+      <c r="L4" s="51">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="M4" s="51">
+        <v>0.193</v>
+      </c>
+      <c r="N4" s="51">
+        <v>0.16300000000000001</v>
+      </c>
+      <c r="O4" s="51">
+        <v>0.36399999999999999</v>
+      </c>
+      <c r="P4" s="51">
+        <v>0.186</v>
+      </c>
+      <c r="Q4" s="51">
+        <v>0.185</v>
+      </c>
+      <c r="R4" s="51">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="S4" s="51">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="T4" s="49">
+        <v>-1.2E-2</v>
+      </c>
+      <c r="U4" s="49">
+        <v>-1.2E-2</v>
+      </c>
+      <c r="V4" s="49">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="W4" s="48">
+        <v>0.11600000000000001</v>
+      </c>
+      <c r="X4" s="48">
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="Y4" s="49">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="Z4" s="49">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="AA4" s="49">
+        <v>0.17599999999999999</v>
+      </c>
+      <c r="AB4" s="48">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="AC4" s="49">
+        <v>0.45500000000000002</v>
+      </c>
+      <c r="AD4" s="49">
+        <v>0.17599999999999999</v>
+      </c>
+      <c r="AE4" s="49">
+        <v>-2.4E-2</v>
+      </c>
+      <c r="AF4" s="49">
+        <v>4.7E-2</v>
+      </c>
+      <c r="AG4" s="49">
+        <v>4.7E-2</v>
+      </c>
+      <c r="AH4" s="49">
+        <v>4.7E-2</v>
+      </c>
+      <c r="AI4" s="49">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AJ4" s="49">
+        <v>0.39400000000000002</v>
+      </c>
+      <c r="AK4" s="49">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="AL4" s="49">
+        <v>0.255</v>
+      </c>
+      <c r="AM4" s="48">
+        <v>0.10100000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:39" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="6">
+        <v>2003</v>
+      </c>
+      <c r="B5" s="47">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="C5" s="48">
+        <v>-3.1E-2</v>
+      </c>
+      <c r="D5" s="49">
+        <v>-3.6999999999999998E-2</v>
+      </c>
+      <c r="E5" s="49">
+        <v>-0.16400000000000001</v>
+      </c>
+      <c r="F5" s="49">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="G5" s="49">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="H5" s="49">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="I5" s="48">
+        <v>4.7E-2</v>
+      </c>
+      <c r="J5" s="49">
+        <v>-0.20499999999999999</v>
+      </c>
+      <c r="K5" s="50">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="L5" s="51">
+        <v>0.115</v>
+      </c>
+      <c r="M5" s="51">
+        <v>-9.2999999999999999E-2</v>
+      </c>
+      <c r="N5" s="51">
+        <v>0.106</v>
+      </c>
+      <c r="O5" s="51">
+        <v>0.35299999999999998</v>
+      </c>
+      <c r="P5" s="51">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="Q5" s="51">
+        <v>0.08</v>
+      </c>
+      <c r="R5" s="51">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="S5" s="51">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="T5" s="49">
+        <v>-9.4E-2</v>
+      </c>
+      <c r="U5" s="49">
+        <v>-9.4E-2</v>
+      </c>
+      <c r="V5" s="49">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="W5" s="48">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="X5" s="48">
+        <v>0.03</v>
+      </c>
+      <c r="Y5" s="49">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="Z5" s="49">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="AA5" s="49">
+        <v>6.3E-2</v>
+      </c>
+      <c r="AB5" s="48">
+        <v>9.4E-2</v>
+      </c>
+      <c r="AC5" s="49">
+        <v>0.50700000000000001</v>
+      </c>
+      <c r="AD5" s="49">
+        <v>6.3E-2</v>
+      </c>
+      <c r="AE5" s="49">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="AF5" s="49">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="AG5" s="49">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="AH5" s="49">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="AI5" s="49">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="AJ5" s="49">
+        <v>-0.05</v>
+      </c>
+      <c r="AK5" s="49">
+        <v>0.20100000000000001</v>
+      </c>
+      <c r="AL5" s="49">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="AM5" s="48">
+        <v>-5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:39" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="6">
+        <v>2004</v>
+      </c>
+      <c r="B6" s="47">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="C6" s="48">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="D6" s="49">
+        <v>-4.0000000000000001E-3</v>
+      </c>
+      <c r="E6" s="49">
+        <v>0.62</v>
+      </c>
+      <c r="F6" s="49">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="G6" s="49">
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="H6" s="49">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="I6" s="48">
+        <v>0.155</v>
+      </c>
+      <c r="J6" s="49">
+        <v>0.496</v>
+      </c>
+      <c r="K6" s="50">
+        <v>0.123</v>
+      </c>
+      <c r="L6" s="51">
+        <v>0.35799999999999998</v>
+      </c>
+      <c r="M6" s="51">
+        <v>2.3E-2</v>
+      </c>
+      <c r="N6" s="51">
+        <v>0.186</v>
+      </c>
+      <c r="O6" s="51">
+        <v>0.113</v>
+      </c>
+      <c r="P6" s="51">
+        <v>9.7000000000000003E-2</v>
+      </c>
+      <c r="Q6" s="51">
+        <v>3.1E-2</v>
+      </c>
+      <c r="R6" s="51">
+        <v>-7.1999999999999995E-2</v>
+      </c>
+      <c r="S6" s="51">
+        <v>-7.1999999999999995E-2</v>
+      </c>
+      <c r="T6" s="49">
+        <v>-0.32500000000000001</v>
+      </c>
+      <c r="U6" s="49">
+        <v>-0.32500000000000001</v>
+      </c>
+      <c r="V6" s="49">
+        <v>0.2</v>
+      </c>
+      <c r="W6" s="48">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="X6" s="48">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="Y6" s="49">
+        <v>0.125</v>
+      </c>
+      <c r="Z6" s="49">
+        <v>0.125</v>
+      </c>
+      <c r="AA6" s="49">
+        <v>0.183</v>
+      </c>
+      <c r="AB6" s="48">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="AC6" s="49">
+        <v>0.26300000000000001</v>
+      </c>
+      <c r="AD6" s="49">
+        <v>0.183</v>
+      </c>
+      <c r="AE6" s="49">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="AF6" s="49">
+        <v>2.7E-2</v>
+      </c>
+      <c r="AG6" s="49">
+        <v>2.7E-2</v>
+      </c>
+      <c r="AH6" s="49">
+        <v>2.7E-2</v>
+      </c>
+      <c r="AI6" s="49">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="AJ6" s="49">
+        <v>0.19400000000000001</v>
+      </c>
+      <c r="AK6" s="49">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="AL6" s="49">
+        <v>0.159</v>
+      </c>
+      <c r="AM6" s="48">
+        <v>4.4999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:39" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="6">
+        <v>2005</v>
+      </c>
+      <c r="B7" s="47">
+        <v>9.4E-2</v>
+      </c>
+      <c r="C7" s="48">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="D7" s="49">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="E7" s="49">
+        <v>-0.22500000000000001</v>
+      </c>
+      <c r="F7" s="49">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="G7" s="49">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="H7" s="49">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="I7" s="48">
+        <v>9.2999999999999999E-2</v>
+      </c>
+      <c r="J7" s="49">
+        <v>0.30399999999999999</v>
+      </c>
+      <c r="K7" s="50">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="L7" s="51">
+        <v>0.122</v>
+      </c>
+      <c r="M7" s="51">
+        <v>0.114</v>
+      </c>
+      <c r="N7" s="51">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="O7" s="51">
+        <v>0.35599999999999998</v>
+      </c>
+      <c r="P7" s="51">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="Q7" s="51">
+        <v>2E-3</v>
+      </c>
+      <c r="R7" s="51">
+        <v>-0.17899999999999999</v>
+      </c>
+      <c r="S7" s="51">
+        <v>-0.17899999999999999</v>
+      </c>
+      <c r="T7" s="49">
+        <v>-0.111</v>
+      </c>
+      <c r="U7" s="49">
+        <v>-0.111</v>
+      </c>
+      <c r="V7" s="49">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="W7" s="48">
+        <v>0.11899999999999999</v>
+      </c>
+      <c r="X7" s="48">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="Y7" s="49">
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="Z7" s="49">
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="AA7" s="49">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="AB7" s="48">
+        <v>0.114</v>
+      </c>
+      <c r="AC7" s="49">
+        <v>0.36599999999999999</v>
+      </c>
+      <c r="AD7" s="49">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="AE7" s="49">
+        <v>1.4E-2</v>
+      </c>
+      <c r="AF7" s="49">
+        <v>8.1000000000000003E-2</v>
+      </c>
+      <c r="AG7" s="49">
+        <v>8.1000000000000003E-2</v>
+      </c>
+      <c r="AH7" s="49">
+        <v>8.1000000000000003E-2</v>
+      </c>
+      <c r="AI7" s="49">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="AJ7" s="49">
+        <v>0.183</v>
+      </c>
+      <c r="AK7" s="49">
+        <v>-3.3000000000000002E-2</v>
+      </c>
+      <c r="AL7" s="49">
+        <v>0.34300000000000003</v>
+      </c>
+      <c r="AM7" s="48">
+        <v>6.3E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:39" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="6">
+        <v>2006</v>
+      </c>
+      <c r="B8" s="47">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="C8" s="48">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="D8" s="49">
+        <v>1.4E-2</v>
+      </c>
+      <c r="E8" s="49">
+        <v>0.32800000000000001</v>
+      </c>
+      <c r="F8" s="49">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="G8" s="49">
+        <v>0.08</v>
+      </c>
+      <c r="H8" s="49">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="I8" s="48">
+        <v>0.11700000000000001</v>
+      </c>
+      <c r="J8" s="49">
+        <v>-0.13800000000000001</v>
+      </c>
+      <c r="K8" s="50">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="L8" s="51">
+        <v>0.16300000000000001</v>
+      </c>
+      <c r="M8" s="51">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="N8" s="51">
+        <v>0.153</v>
+      </c>
+      <c r="O8" s="51">
+        <v>0.22700000000000001</v>
+      </c>
+      <c r="P8" s="51">
+        <v>0.187</v>
+      </c>
+      <c r="Q8" s="51">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="R8" s="51">
+        <v>0.214</v>
+      </c>
+      <c r="S8" s="51">
+        <v>0.214</v>
+      </c>
+      <c r="T8" s="49">
+        <v>-0.13</v>
+      </c>
+      <c r="U8" s="49">
+        <v>-0.13</v>
+      </c>
+      <c r="V8" s="49">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="W8" s="48">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="X8" s="48">
+        <v>0.20599999999999999</v>
+      </c>
+      <c r="Y8" s="49">
+        <v>0.182</v>
+      </c>
+      <c r="Z8" s="49">
+        <v>0.182</v>
+      </c>
+      <c r="AA8" s="49">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="AB8" s="48">
+        <v>2.7E-2</v>
+      </c>
+      <c r="AC8" s="49">
+        <v>0.22800000000000001</v>
+      </c>
+      <c r="AD8" s="49">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="AE8" s="49">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="AF8" s="49">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="AG8" s="49">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="AH8" s="49">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="AI8" s="49">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="AJ8" s="49">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="AK8" s="49">
+        <v>0.08</v>
+      </c>
+      <c r="AL8" s="49">
+        <v>0.19400000000000001</v>
+      </c>
+      <c r="AM8" s="48">
+        <v>8.6999999999999994E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:39" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="6">
+        <v>2007</v>
+      </c>
+      <c r="B9" s="47">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="C9" s="48">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="D9" s="49">
+        <v>0.04</v>
+      </c>
+      <c r="E9" s="49">
+        <v>-0.29199999999999998</v>
+      </c>
+      <c r="F9" s="49">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="G9" s="49">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="H9" s="49">
+        <v>2.7E-2</v>
+      </c>
+      <c r="I9" s="48">
+        <v>0.09</v>
+      </c>
+      <c r="J9" s="49">
+        <v>0.42799999999999999</v>
+      </c>
+      <c r="K9" s="50">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="L9" s="51">
+        <v>-4.4999999999999998E-2</v>
+      </c>
+      <c r="M9" s="51">
+        <v>-1.6E-2</v>
+      </c>
+      <c r="N9" s="51">
+        <v>0.09</v>
+      </c>
+      <c r="O9" s="51">
+        <v>0.17799999999999999</v>
+      </c>
+      <c r="P9" s="51">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="Q9" s="51">
+        <v>0.01</v>
+      </c>
+      <c r="R9" s="51">
+        <v>0.218</v>
+      </c>
+      <c r="S9" s="51">
+        <v>0.218</v>
+      </c>
+      <c r="T9" s="49">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="U9" s="49">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="V9" s="49">
+        <v>0.14899999999999999</v>
+      </c>
+      <c r="W9" s="48">
+        <v>0.122</v>
+      </c>
+      <c r="X9" s="48">
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="Y9" s="49">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="Z9" s="49">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="AA9" s="49">
+        <v>0.15</v>
+      </c>
+      <c r="AB9" s="48">
+        <v>0.108</v>
+      </c>
+      <c r="AC9" s="49">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="AD9" s="49">
+        <v>0.14899999999999999</v>
+      </c>
+      <c r="AE9" s="49">
+        <v>0.11600000000000001</v>
+      </c>
+      <c r="AF9" s="49">
+        <v>0.107</v>
+      </c>
+      <c r="AG9" s="49">
+        <v>0.107</v>
+      </c>
+      <c r="AH9" s="49">
+        <v>0.107</v>
+      </c>
+      <c r="AI9" s="49">
+        <v>0.06</v>
+      </c>
+      <c r="AJ9" s="49">
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="AK9" s="49">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="AL9" s="49">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="AM9" s="48">
+        <v>4.3999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:39" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="6">
+        <v>2008</v>
+      </c>
+      <c r="B10" s="47">
+        <v>0.112</v>
+      </c>
+      <c r="C10" s="48">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="D10" s="49">
+        <v>6.2E-2</v>
+      </c>
+      <c r="E10" s="49">
+        <v>0.29299999999999998</v>
+      </c>
+      <c r="F10" s="49">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="G10" s="49">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="H10" s="49">
+        <v>2.7E-2</v>
+      </c>
+      <c r="I10" s="48">
+        <v>0.151</v>
+      </c>
+      <c r="J10" s="49">
+        <v>-0.157</v>
+      </c>
+      <c r="K10" s="50">
+        <v>5.5E-2</v>
+      </c>
+      <c r="L10" s="51">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="M10" s="51">
+        <v>0.03</v>
+      </c>
+      <c r="N10" s="51">
+        <v>-1.4E-2</v>
+      </c>
+      <c r="O10" s="51">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="P10" s="51">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="Q10" s="51">
+        <v>0.05</v>
+      </c>
+      <c r="R10" s="51">
+        <v>0.109</v>
+      </c>
+      <c r="S10" s="51">
+        <v>0.109</v>
+      </c>
+      <c r="T10" s="49">
+        <v>0.18099999999999999</v>
+      </c>
+      <c r="U10" s="49">
+        <v>0.18099999999999999</v>
+      </c>
+      <c r="V10" s="49">
+        <v>0.28199999999999997</v>
+      </c>
+      <c r="W10" s="48">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="X10" s="48">
+        <v>0.20599999999999999</v>
+      </c>
+      <c r="Y10" s="49">
+        <v>0.19400000000000001</v>
+      </c>
+      <c r="Z10" s="49">
+        <v>0.19400000000000001</v>
+      </c>
+      <c r="AA10" s="49">
+        <v>0.23799999999999999</v>
+      </c>
+      <c r="AB10" s="48">
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="AC10" s="49">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="AD10" s="49">
+        <v>0.23</v>
+      </c>
+      <c r="AE10" s="49">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="AF10" s="49">
+        <v>0.155</v>
+      </c>
+      <c r="AG10" s="49">
+        <v>0.155</v>
+      </c>
+      <c r="AH10" s="49">
+        <v>0.155</v>
+      </c>
+      <c r="AI10" s="49">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="AJ10" s="49">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="AK10" s="49">
+        <v>0.11899999999999999</v>
+      </c>
+      <c r="AL10" s="49">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="AM10" s="48">
+        <v>0.115</v>
+      </c>
+    </row>
+    <row r="11" spans="1:39" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="6">
+        <v>2009</v>
+      </c>
+      <c r="B11" s="47">
+        <v>6.2E-2</v>
+      </c>
+      <c r="C11" s="48">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="D11" s="49">
+        <v>9.4E-2</v>
+      </c>
+      <c r="E11" s="49">
+        <v>-0.153</v>
+      </c>
+      <c r="F11" s="49">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="G11" s="49">
+        <v>2.4E-2</v>
+      </c>
+      <c r="H11" s="49">
+        <v>2.7E-2</v>
+      </c>
+      <c r="I11" s="48">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J11" s="49">
+        <v>-0.17899999999999999</v>
+      </c>
+      <c r="K11" s="50">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="L11" s="51">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="M11" s="51">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="N11" s="51">
+        <v>-2.1999999999999999E-2</v>
+      </c>
+      <c r="O11" s="51">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="P11" s="51">
+        <v>1E-3</v>
+      </c>
+      <c r="Q11" s="51">
+        <v>-5.5E-2</v>
+      </c>
+      <c r="R11" s="51">
+        <v>-0.05</v>
+      </c>
+      <c r="S11" s="51">
+        <v>-0.05</v>
+      </c>
+      <c r="T11" s="49">
+        <v>0.14599999999999999</v>
+      </c>
+      <c r="U11" s="49">
+        <v>0.14599999999999999</v>
+      </c>
+      <c r="V11" s="49">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="W11" s="48">
+        <v>6.2E-2</v>
+      </c>
+      <c r="X11" s="48">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="Y11" s="49">
+        <v>0.04</v>
+      </c>
+      <c r="Z11" s="49">
+        <v>0.04</v>
+      </c>
+      <c r="AA11" s="49">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="AB11" s="48">
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="AC11" s="49">
+        <v>-5.8000000000000003E-2</v>
+      </c>
+      <c r="AD11" s="49">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="AE11" s="49">
+        <v>-4.1000000000000002E-2</v>
+      </c>
+      <c r="AF11" s="49">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="AG11" s="49">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="AH11" s="49">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="AI11" s="49">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="AJ11" s="49">
+        <v>0.155</v>
+      </c>
+      <c r="AK11" s="49">
+        <v>0.151</v>
+      </c>
+      <c r="AL11" s="49">
+        <v>-5.2999999999999999E-2</v>
+      </c>
+      <c r="AM11" s="48">
+        <v>9.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:39" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="6">
+        <v>2010</v>
+      </c>
+      <c r="B12" s="47">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="C12" s="48">
+        <v>0.05</v>
+      </c>
+      <c r="D12" s="49">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="E12" s="49">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="F12" s="49">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="G12" s="49">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="H12" s="49">
+        <v>2.7E-2</v>
+      </c>
+      <c r="I12" s="48">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="J12" s="49">
+        <v>-0.108</v>
+      </c>
+      <c r="K12" s="50">
+        <v>9.2999999999999999E-2</v>
+      </c>
+      <c r="L12" s="51">
+        <v>9.2999999999999999E-2</v>
+      </c>
+      <c r="M12" s="51">
+        <v>0.02</v>
+      </c>
+      <c r="N12" s="51">
+        <v>2.4E-2</v>
+      </c>
+      <c r="O12" s="51">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="P12" s="51">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="Q12" s="51">
+        <v>0.108</v>
+      </c>
+      <c r="R12" s="51">
+        <v>0.437</v>
+      </c>
+      <c r="S12" s="51">
+        <v>0.437</v>
+      </c>
+      <c r="T12" s="49">
+        <v>0.153</v>
+      </c>
+      <c r="U12" s="49">
+        <v>0.153</v>
+      </c>
+      <c r="V12" s="49">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="W12" s="48">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="X12" s="48">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="Y12" s="49">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="Z12" s="49">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="AA12" s="49">
+        <v>0.09</v>
+      </c>
+      <c r="AB12" s="48">
+        <v>9.2999999999999999E-2</v>
+      </c>
+      <c r="AC12" s="49">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="AD12" s="49">
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="AE12" s="49">
+        <v>0.23599999999999999</v>
+      </c>
+      <c r="AF12" s="49">
+        <v>0.01</v>
+      </c>
+      <c r="AG12" s="49">
+        <v>0.01</v>
+      </c>
+      <c r="AH12" s="49">
+        <v>0.01</v>
+      </c>
+      <c r="AI12" s="49">
+        <v>0.14399999999999999</v>
+      </c>
+      <c r="AJ12" s="49">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="AK12" s="49">
+        <v>0.157</v>
+      </c>
+      <c r="AL12" s="49">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AM12" s="48">
+        <v>4.9000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:39" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="6">
+        <v>2011</v>
+      </c>
+      <c r="B13" s="47">
+        <v>0.08</v>
+      </c>
+      <c r="C13" s="48">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="D13" s="49">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="E13" s="49">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="F13" s="49">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="G13" s="49">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="H13" s="49">
+        <v>2.7E-2</v>
+      </c>
+      <c r="I13" s="48">
+        <v>0.17799999999999999</v>
+      </c>
+      <c r="J13" s="49">
+        <v>0.497</v>
+      </c>
+      <c r="K13" s="50">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="L13" s="51">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="M13" s="51">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="N13" s="51">
+        <v>-1.4E-2</v>
+      </c>
+      <c r="O13" s="51">
+        <v>-0.108</v>
+      </c>
+      <c r="P13" s="51">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="Q13" s="51">
+        <v>0.17899999999999999</v>
+      </c>
+      <c r="R13" s="51">
+        <v>0.33400000000000002</v>
+      </c>
+      <c r="S13" s="51">
+        <v>0.33400000000000002</v>
+      </c>
+      <c r="T13" s="49">
+        <v>0.152</v>
+      </c>
+      <c r="U13" s="49">
+        <v>0.152</v>
+      </c>
+      <c r="V13" s="49">
+        <v>0.23599999999999999</v>
+      </c>
+      <c r="W13" s="48">
+        <v>0.08</v>
+      </c>
+      <c r="X13" s="48">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="Y13" s="49">
+        <v>7.8E-2</v>
+      </c>
+      <c r="Z13" s="49">
+        <v>7.8E-2</v>
+      </c>
+      <c r="AA13" s="49">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="AB13" s="48">
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="AC13" s="49">
+        <v>3.9E-2</v>
+      </c>
+      <c r="AD13" s="49">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="AE13" s="49">
+        <v>0.20300000000000001</v>
+      </c>
+      <c r="AF13" s="49">
+        <v>-2E-3</v>
+      </c>
+      <c r="AG13" s="49">
+        <v>-2E-3</v>
+      </c>
+      <c r="AH13" s="49">
+        <v>-2E-3</v>
+      </c>
+      <c r="AI13" s="49">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="AJ13" s="49">
+        <v>0.18</v>
+      </c>
+      <c r="AK13" s="49">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="AL13" s="49">
+        <v>-7.0000000000000001E-3</v>
+      </c>
+      <c r="AM13" s="48">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:39" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="6">
+        <v>2012</v>
+      </c>
+      <c r="B14" s="47">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="C14" s="48">
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="D14" s="49">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="E14" s="49">
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="F14" s="49">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="G14" s="49">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="H14" s="49">
+        <v>-2.3E-2</v>
+      </c>
+      <c r="I14" s="48">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="J14" s="49">
+        <v>-7.0999999999999994E-2</v>
+      </c>
+      <c r="K14" s="50">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="L14" s="51">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="M14" s="51">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="N14" s="51">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="O14" s="51">
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="P14" s="51">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="Q14" s="51">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="R14" s="51">
+        <v>0.25900000000000001</v>
+      </c>
+      <c r="S14" s="51">
+        <v>9.7000000000000003E-2</v>
+      </c>
+      <c r="T14" s="49">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="U14" s="49">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="V14" s="49">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="W14" s="48">
+        <v>0.11600000000000001</v>
+      </c>
+      <c r="X14" s="48">
+        <v>0.14899999999999999</v>
+      </c>
+      <c r="Y14" s="49">
+        <v>0.08</v>
+      </c>
+      <c r="Z14" s="49">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="AA14" s="49">
+        <v>0.19</v>
+      </c>
+      <c r="AB14" s="48">
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="AC14" s="49">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="AD14" s="49">
+        <v>0.32900000000000001</v>
+      </c>
+      <c r="AE14" s="49">
+        <v>0.126</v>
+      </c>
+      <c r="AF14" s="49">
+        <v>-3.0000000000000001E-3</v>
+      </c>
+      <c r="AG14" s="49">
+        <v>0.06</v>
+      </c>
+      <c r="AH14" s="49">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="AI14" s="49">
+        <v>0.218</v>
+      </c>
+      <c r="AJ14" s="49">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="AK14" s="49">
+        <v>0.23200000000000001</v>
+      </c>
+      <c r="AL14" s="49">
+        <v>0.109</v>
+      </c>
+      <c r="AM14" s="48">
+        <v>1.9E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:39" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="6">
+        <v>2013</v>
+      </c>
+      <c r="B15" s="47">
+        <v>4.7E-2</v>
+      </c>
+      <c r="C15" s="48">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="D15" s="49">
+        <v>3.9E-2</v>
+      </c>
+      <c r="E15" s="49">
+        <v>-4.8000000000000001E-2</v>
+      </c>
+      <c r="F15" s="49">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="G15" s="49">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="H15" s="49">
+        <v>4.7E-2</v>
+      </c>
+      <c r="I15" s="48">
+        <v>9.4E-2</v>
+      </c>
+      <c r="J15" s="49">
+        <v>0.19600000000000001</v>
+      </c>
+      <c r="K15" s="50">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="L15" s="51">
+        <v>8.1000000000000003E-2</v>
+      </c>
+      <c r="M15" s="51">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="N15" s="51">
+        <v>-0.77900000000000003</v>
+      </c>
+      <c r="O15" s="51">
+        <v>0.124</v>
+      </c>
+      <c r="P15" s="51">
+        <v>-3.3000000000000002E-2</v>
+      </c>
+      <c r="Q15" s="51">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="R15" s="51">
+        <v>-0.13900000000000001</v>
+      </c>
+      <c r="S15" s="51">
+        <v>0.11899999999999999</v>
+      </c>
+      <c r="T15" s="49">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="U15" s="49">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="V15" s="49">
+        <v>0.108</v>
+      </c>
+      <c r="W15" s="48">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="X15" s="48">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="Y15" s="49">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="Z15" s="49">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="AA15" s="49">
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="AB15" s="48">
+        <v>0.05</v>
+      </c>
+      <c r="AC15" s="49">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="AD15" s="49">
+        <v>-4.0000000000000001E-3</v>
+      </c>
+      <c r="AE15" s="49">
+        <v>0.1</v>
+      </c>
+      <c r="AF15" s="49">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="AG15" s="49">
+        <v>3.9E-2</v>
+      </c>
+      <c r="AH15" s="49">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="AI15" s="49">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="AJ15" s="49">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="AK15" s="49">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="AL15" s="49">
+        <v>0.124</v>
+      </c>
+      <c r="AM15" s="48">
+        <v>-3.2000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:39" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="6">
+        <v>2014</v>
+      </c>
+      <c r="B16" s="47">
+        <v>6.2E-2</v>
+      </c>
+      <c r="C16" s="48">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="D16" s="49">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="E16" s="49">
+        <v>-0.02</v>
+      </c>
+      <c r="F16" s="49">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="G16" s="49">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="H16" s="49">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="I16" s="48">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="J16" s="49">
+        <v>0.252</v>
+      </c>
+      <c r="K16" s="50">
+        <v>-0.126</v>
+      </c>
+      <c r="L16" s="51">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="M16" s="51">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="N16" s="51">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="O16" s="51">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="P16" s="51">
+        <v>-1.6E-2</v>
+      </c>
+      <c r="Q16" s="51">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="R16" s="51">
+        <v>0.29299999999999998</v>
+      </c>
+      <c r="S16" s="51">
+        <v>0.13</v>
+      </c>
+      <c r="T16" s="49">
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="U16" s="49">
+        <v>0.03</v>
+      </c>
+      <c r="V16" s="49">
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="W16" s="48">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="X16" s="48">
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="Y16" s="49">
+        <v>0.04</v>
+      </c>
+      <c r="Z16" s="49">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="AA16" s="49">
+        <v>0.04</v>
+      </c>
+      <c r="AB16" s="48">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AC16" s="49">
+        <v>0.123</v>
+      </c>
+      <c r="AD16" s="49">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="AE16" s="49">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="AF16" s="49">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="AG16" s="49">
+        <v>-7.4999999999999997E-2</v>
+      </c>
+      <c r="AH16" s="49">
+        <v>0.14899999999999999</v>
+      </c>
+      <c r="AI16" s="49">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="AJ16" s="49">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="AK16" s="49">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="AL16" s="49">
+        <v>0.161</v>
+      </c>
+      <c r="AM16" s="48">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="17" spans="1:39" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="6">
+        <v>2015</v>
+      </c>
+      <c r="B17" s="47">
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="C17" s="48">
+        <v>0.05</v>
+      </c>
+      <c r="D17" s="49">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="E17" s="49">
+        <v>0.14399999999999999</v>
+      </c>
+      <c r="F17" s="49">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="G17" s="49">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="H17" s="49">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="I17" s="48">
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="J17" s="49">
+        <v>-0.05</v>
+      </c>
+      <c r="K17" s="50">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="L17" s="51">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="M17" s="51">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="N17" s="51">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="O17" s="51">
+        <v>0.107</v>
+      </c>
+      <c r="P17" s="51">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="Q17" s="51">
+        <v>0.19700000000000001</v>
+      </c>
+      <c r="R17" s="51">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="S17" s="51">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="T17" s="49">
+        <v>0.08</v>
+      </c>
+      <c r="U17" s="49">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="V17" s="49">
+        <v>0.154</v>
+      </c>
+      <c r="W17" s="48">
+        <v>0.104</v>
+      </c>
+      <c r="X17" s="48">
+        <v>0.115</v>
+      </c>
+      <c r="Y17" s="49">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="Z17" s="49">
+        <v>0.127</v>
+      </c>
+      <c r="AA17" s="49">
+        <v>9.7000000000000003E-2</v>
+      </c>
+      <c r="AB17" s="48">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="AC17" s="49">
+        <v>9.2999999999999999E-2</v>
+      </c>
+      <c r="AD17" s="49">
+        <v>0.17899999999999999</v>
+      </c>
+      <c r="AE17" s="49">
+        <v>0.122</v>
+      </c>
+      <c r="AF17" s="49">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="AG17" s="49">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="AH17" s="49">
+        <v>0.161</v>
+      </c>
+      <c r="AI17" s="49">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="AJ17" s="49">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="AK17" s="49">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="AL17" s="49">
+        <v>0.192</v>
+      </c>
+      <c r="AM17" s="48">
+        <v>0.14099999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:39" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="6">
+        <v>2016</v>
+      </c>
+      <c r="B18" s="47">
+        <v>0.06</v>
+      </c>
+      <c r="C18" s="48">
+        <v>3.9E-2</v>
+      </c>
+      <c r="D18" s="49">
+        <v>0.03</v>
+      </c>
+      <c r="E18" s="49">
+        <v>2.4E-2</v>
+      </c>
+      <c r="F18" s="49">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="G18" s="49">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="H18" s="49">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="I18" s="48">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="J18" s="49">
+        <v>0.104</v>
+      </c>
+      <c r="K18" s="50">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="L18" s="51">
+        <v>8.1000000000000003E-2</v>
+      </c>
+      <c r="M18" s="51">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="N18" s="51">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="O18" s="51">
+        <v>0.106</v>
+      </c>
+      <c r="P18" s="51">
+        <v>0.05</v>
+      </c>
+      <c r="Q18" s="51">
+        <v>0.21099999999999999</v>
+      </c>
+      <c r="R18" s="51">
+        <v>0.16</v>
+      </c>
+      <c r="S18" s="51">
+        <v>-9.7000000000000003E-2</v>
+      </c>
+      <c r="T18" s="49">
+        <v>0.13700000000000001</v>
+      </c>
+      <c r="U18" s="49">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="V18" s="49">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="W18" s="48">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="X18" s="48">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="Y18" s="49">
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="Z18" s="49">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="AA18" s="49">
+        <v>0.08</v>
+      </c>
+      <c r="AB18" s="48">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="AC18" s="49">
+        <v>0.113</v>
+      </c>
+      <c r="AD18" s="49">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="AE18" s="49">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="AF18" s="49">
+        <v>6.2E-2</v>
+      </c>
+      <c r="AG18" s="49">
+        <v>6.3E-2</v>
+      </c>
+      <c r="AH18" s="49">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="AI18" s="49">
+        <v>0.114</v>
+      </c>
+      <c r="AJ18" s="49">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="AK18" s="49">
+        <v>6.2E-2</v>
+      </c>
+      <c r="AL18" s="49">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AM18" s="48">
+        <v>4.4999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:39" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="6">
+        <v>2017</v>
+      </c>
+      <c r="B19" s="47">
+        <v>3.9E-2</v>
+      </c>
+      <c r="C19" s="48">
+        <v>4.7E-2</v>
+      </c>
+      <c r="D19" s="49">
+        <v>0.05</v>
+      </c>
+      <c r="E19" s="49">
+        <v>1.6E-2</v>
+      </c>
+      <c r="F19" s="49">
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="G19" s="49">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="H19" s="49">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="I19" s="48">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="J19" s="49">
+        <v>0.2</v>
+      </c>
+      <c r="K19" s="50">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="L19" s="51">
+        <v>0.12</v>
+      </c>
+      <c r="M19" s="51">
+        <v>-8.2000000000000003E-2</v>
+      </c>
+      <c r="N19" s="51">
+        <v>0.39500000000000002</v>
+      </c>
+      <c r="O19" s="51">
+        <v>-7.9000000000000001E-2</v>
+      </c>
+      <c r="P19" s="51">
+        <v>0.32800000000000001</v>
+      </c>
+      <c r="Q19" s="51">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="R19" s="51">
+        <v>0.111</v>
+      </c>
+      <c r="S19" s="51">
+        <v>0.112</v>
+      </c>
+      <c r="T19" s="49">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="U19" s="49">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="V19" s="49">
+        <v>-9.8000000000000004E-2</v>
+      </c>
+      <c r="W19" s="48">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="X19" s="48">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="Y19" s="49">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="Z19" s="49">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="AA19" s="49">
+        <v>0.151</v>
+      </c>
+      <c r="AB19" s="48">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="AC19" s="49">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="AD19" s="49">
+        <v>0.105</v>
+      </c>
+      <c r="AE19" s="49">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="AF19" s="49">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AG19" s="49">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="AH19" s="49">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="AI19" s="49">
+        <v>0.02</v>
+      </c>
+      <c r="AJ19" s="49">
+        <v>2.3E-2</v>
+      </c>
+      <c r="AK19" s="49">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="AL19" s="49">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="AM19" s="48">
+        <v>-2.4E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:39" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="6">
+        <v>2018</v>
+      </c>
+      <c r="B20" s="47">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="C20" s="48">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="D20" s="49">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="E20" s="49">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="F20" s="49">
+        <v>0.107</v>
+      </c>
+      <c r="G20" s="49">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="H20" s="49">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="I20" s="48">
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="J20" s="49">
+        <v>3.1E-2</v>
+      </c>
+      <c r="K20" s="50">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="L20" s="51">
+        <v>0.128</v>
+      </c>
+      <c r="M20" s="51">
+        <v>3.9E-2</v>
+      </c>
+      <c r="N20" s="51">
+        <v>0.59699999999999998</v>
+      </c>
+      <c r="O20" s="51">
+        <v>0.127</v>
+      </c>
+      <c r="P20" s="51">
+        <v>0.187</v>
+      </c>
+      <c r="Q20" s="51">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="R20" s="51">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="S20" s="51">
+        <v>0.105</v>
+      </c>
+      <c r="T20" s="49">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="U20" s="49">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="V20" s="49">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="W20" s="48">
+        <v>9.7000000000000003E-2</v>
+      </c>
+      <c r="X20" s="48">
+        <v>0.182</v>
+      </c>
+      <c r="Y20" s="49">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="Z20" s="49">
+        <v>0.18099999999999999</v>
+      </c>
+      <c r="AA20" s="49">
+        <v>0.19700000000000001</v>
+      </c>
+      <c r="AB20" s="48">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="AC20" s="49">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="AD20" s="49">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="AE20" s="49">
+        <v>0.1</v>
+      </c>
+      <c r="AF20" s="49">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="AG20" s="49">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="AH20" s="49">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="AI20" s="49">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AJ20" s="49">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="AK20" s="49">
+        <v>-2E-3</v>
+      </c>
+      <c r="AL20" s="49">
+        <v>9.2999999999999999E-2</v>
+      </c>
+      <c r="AM20" s="48">
+        <v>9.0999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:39" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="6">
+        <v>2019</v>
+      </c>
+      <c r="B21" s="47">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="C21" s="48">
+        <v>0.05</v>
+      </c>
+      <c r="D21" s="49">
+        <v>0.04</v>
+      </c>
+      <c r="E21" s="49">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="F21" s="49">
+        <v>0.112</v>
+      </c>
+      <c r="G21" s="49">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="H21" s="49">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="I21" s="48">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="J21" s="49">
+        <v>-3.0000000000000001E-3</v>
+      </c>
+      <c r="K21" s="50">
+        <v>0.113</v>
+      </c>
+      <c r="L21" s="51">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="M21" s="51">
+        <v>0.109</v>
+      </c>
+      <c r="N21" s="51">
+        <v>0.183</v>
+      </c>
+      <c r="O21" s="51">
+        <v>0.27100000000000002</v>
+      </c>
+      <c r="P21" s="51">
+        <v>0.313</v>
+      </c>
+      <c r="Q21" s="51">
+        <v>0.188</v>
+      </c>
+      <c r="R21" s="51">
+        <v>0.20300000000000001</v>
+      </c>
+      <c r="S21" s="51">
+        <v>2.7E-2</v>
+      </c>
+      <c r="T21" s="49">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="U21" s="49">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="V21" s="49">
+        <v>0.32800000000000001</v>
+      </c>
+      <c r="W21" s="48">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="X21" s="48">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="Y21" s="49">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="Z21" s="49">
+        <v>0.157</v>
+      </c>
+      <c r="AA21" s="49">
+        <v>0.124</v>
+      </c>
+      <c r="AB21" s="48">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="AC21" s="49">
+        <v>9.7000000000000003E-2</v>
+      </c>
+      <c r="AD21" s="49">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="AE21" s="49">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="AF21" s="49">
+        <v>3.9E-2</v>
+      </c>
+      <c r="AG21" s="49">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="AH21" s="49">
+        <v>4.7E-2</v>
+      </c>
+      <c r="AI21" s="49">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="AJ21" s="49">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="AK21" s="49">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="AL21" s="49">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="AM21" s="48">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:39" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="6">
+        <v>2020</v>
+      </c>
+      <c r="B22" s="47">
+        <v>-3.4000000000000002E-2</v>
+      </c>
+      <c r="C22" s="48">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="D22" s="49">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="E22" s="49">
+        <v>-9.4E-2</v>
+      </c>
+      <c r="F22" s="49">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="G22" s="49">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="H22" s="49">
+        <v>-0.155</v>
+      </c>
+      <c r="I22" s="48">
+        <v>-4.2000000000000003E-2</v>
+      </c>
+      <c r="J22" s="49">
+        <v>-0.312</v>
+      </c>
+      <c r="K22" s="50">
+        <v>0.02</v>
+      </c>
+      <c r="L22" s="51">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="M22" s="51">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="N22" s="51">
+        <v>-4.1000000000000002E-2</v>
+      </c>
+      <c r="O22" s="51">
+        <v>-9.0999999999999998E-2</v>
+      </c>
+      <c r="P22" s="51">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="Q22" s="51">
+        <v>-8.0000000000000002E-3</v>
+      </c>
+      <c r="R22" s="51">
+        <v>0.08</v>
+      </c>
+      <c r="S22" s="51">
+        <v>-3.6999999999999998E-2</v>
+      </c>
+      <c r="T22" s="49">
+        <v>1.9E-2</v>
+      </c>
+      <c r="U22" s="49">
+        <v>2.4E-2</v>
+      </c>
+      <c r="V22" s="49">
+        <v>-5.7000000000000002E-2</v>
+      </c>
+      <c r="W22" s="48">
+        <v>-5.5E-2</v>
+      </c>
+      <c r="X22" s="48">
+        <v>-0.106</v>
+      </c>
+      <c r="Y22" s="49">
+        <v>-3.1E-2</v>
+      </c>
+      <c r="Z22" s="49">
+        <v>-3.3000000000000002E-2</v>
+      </c>
+      <c r="AA22" s="49">
+        <v>-0.23699999999999999</v>
+      </c>
+      <c r="AB22" s="48">
+        <v>-3.3000000000000002E-2</v>
+      </c>
+      <c r="AC22" s="49">
+        <v>-0.40200000000000002</v>
+      </c>
+      <c r="AD22" s="49">
+        <v>0.29199999999999998</v>
+      </c>
+      <c r="AE22" s="49">
+        <v>-2.4E-2</v>
+      </c>
+      <c r="AF22" s="49">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="AG22" s="49">
+        <v>-8.0000000000000002E-3</v>
+      </c>
+      <c r="AH22" s="49">
+        <v>-6.8000000000000005E-2</v>
+      </c>
+      <c r="AI22" s="49">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="AJ22" s="49">
+        <v>-0.375</v>
+      </c>
+      <c r="AK22" s="49">
+        <v>0.159</v>
+      </c>
+      <c r="AL22" s="49">
+        <v>-1.2E-2</v>
+      </c>
+      <c r="AM22" s="48">
+        <v>-1.7000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:39" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="6">
+        <v>2021</v>
+      </c>
+      <c r="B23" s="47">
+        <v>0.109</v>
+      </c>
+      <c r="C23" s="48">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="D23" s="49">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="E23" s="49">
+        <v>-5.0000000000000001E-3</v>
+      </c>
+      <c r="F23" s="49">
+        <v>8.1000000000000003E-2</v>
+      </c>
+      <c r="G23" s="49">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="H23" s="49">
+        <v>0.24</v>
+      </c>
+      <c r="I23" s="48">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="J23" s="49">
+        <v>0.26700000000000002</v>
+      </c>
+      <c r="K23" s="50">
+        <v>0.106</v>
+      </c>
+      <c r="L23" s="51">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="M23" s="51">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="N23" s="51">
+        <v>0.156</v>
+      </c>
+      <c r="O23" s="51">
+        <v>0.187</v>
+      </c>
+      <c r="P23" s="51">
+        <v>0.22800000000000001</v>
+      </c>
+      <c r="Q23" s="51">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="R23" s="51">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="S23" s="51">
+        <v>0.23400000000000001</v>
+      </c>
+      <c r="T23" s="49">
+        <v>0.11700000000000001</v>
+      </c>
+      <c r="U23" s="49">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="V23" s="49">
+        <v>0.152</v>
+      </c>
+      <c r="W23" s="48">
+        <v>0.11899999999999999</v>
+      </c>
+      <c r="X23" s="48">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="Y23" s="49">
+        <v>0.35299999999999998</v>
+      </c>
+      <c r="Z23" s="49">
+        <v>0.11700000000000001</v>
+      </c>
+      <c r="AA23" s="49">
+        <v>0.14599999999999999</v>
+      </c>
+      <c r="AB23" s="48">
+        <v>0.112</v>
+      </c>
+      <c r="AC23" s="49">
+        <v>0.20399999999999999</v>
+      </c>
+      <c r="AD23" s="49">
+        <v>0.188</v>
+      </c>
+      <c r="AE23" s="49">
+        <v>0.18</v>
+      </c>
+      <c r="AF23" s="49">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="AG23" s="49">
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="AH23" s="49">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="AI23" s="49">
+        <v>2.4E-2</v>
+      </c>
+      <c r="AJ23" s="49">
+        <v>0.58599999999999997</v>
+      </c>
+      <c r="AK23" s="49">
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="AL23" s="49">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="AM23" s="48">
+        <v>0.13400000000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:39" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="6">
+        <v>2022</v>
+      </c>
+      <c r="B24" s="47">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="C24" s="48">
+        <v>1.6E-2</v>
+      </c>
+      <c r="D24" s="49">
+        <v>-8.9999999999999993E-3</v>
+      </c>
+      <c r="E24" s="49">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="F24" s="49">
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="G24" s="49">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="H24" s="49">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="I24" s="48">
+        <v>0.05</v>
+      </c>
+      <c r="J24" s="49">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="K24" s="50">
+        <v>0.11</v>
+      </c>
+      <c r="L24" s="51">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="M24" s="51">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="N24" s="51">
+        <v>0.20899999999999999</v>
+      </c>
+      <c r="O24" s="51">
+        <v>0.159</v>
+      </c>
+      <c r="P24" s="51">
+        <v>0.14399999999999999</v>
+      </c>
+      <c r="Q24" s="51">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="R24" s="51">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="S24" s="51">
+        <v>-8.0000000000000002E-3</v>
+      </c>
+      <c r="T24" s="49">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="U24" s="49">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="V24" s="49">
+        <v>-5.7000000000000002E-2</v>
+      </c>
+      <c r="W24" s="48">
+        <v>0.122</v>
+      </c>
+      <c r="X24" s="48">
+        <v>0.159</v>
+      </c>
+      <c r="Y24" s="49">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="Z24" s="49">
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="AA24" s="49">
+        <v>0.217</v>
+      </c>
+      <c r="AB24" s="48">
+        <v>0.106</v>
+      </c>
+      <c r="AC24" s="49">
+        <v>0.86899999999999999</v>
+      </c>
+      <c r="AD24" s="49">
+        <v>0.19700000000000001</v>
+      </c>
+      <c r="AE24" s="49">
+        <v>0.10299999999999999</v>
+      </c>
+      <c r="AF24" s="49">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="AG24" s="49">
+        <v>0.01</v>
+      </c>
+      <c r="AH24" s="49">
+        <v>1.4E-2</v>
+      </c>
+      <c r="AI24" s="49">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="AJ24" s="49">
+        <v>0.17399999999999999</v>
+      </c>
+      <c r="AK24" s="49">
+        <v>8.1000000000000003E-2</v>
+      </c>
+      <c r="AL24" s="49">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="AM24" s="48">
+        <v>0.11799999999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:39" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>